<commit_message>
Up to updates for pre-ASTMH v7 Sugungum calibration
</commit_message>
<xml_diff>
--- a/v5-Sugungum/Params.xlsx
+++ b/v5-Sugungum/Params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Malaria-Uganda-PRISM\v5-Sugungum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D512844-59EA-496C-822E-CE9B7450B4F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EBC88D-75D6-4951-8861-800823B7E03D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,10 +507,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -521,10 +521,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>-5</v>
+        <v>0.4</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
@@ -535,10 +535,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>5</v>
@@ -549,10 +549,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>-5</v>
+        <v>0.4</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
@@ -563,10 +563,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -577,10 +577,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>0.3</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -591,10 +591,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>10</v>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>11</v>
@@ -636,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>12</v>
@@ -647,10 +647,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>13</v>

</xml_diff>